<commit_message>
Correct a bug for recognizing i-control software
</commit_message>
<xml_diff>
--- a/Infinite_example.xlsx
+++ b/Infinite_example.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dener\Documents\WorkSpace\BactEXTRACT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1314AFFA-388C-4DE8-8AB1-7DB5129A8650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7662D58-076B-45AC-AE5B-122F8B7253FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -119,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="131">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -489,6 +490,30 @@
   <si>
     <t>End:</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>0 mM</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>50 uM</t>
+  </si>
+  <si>
+    <t>1 mM</t>
+  </si>
+  <si>
+    <t>100 uM</t>
+  </si>
 </sst>
 </file>
 
@@ -571,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -580,6 +605,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DH298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -52683,4 +52711,740 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BACC7B-9F91-452A-9748-7075B77D451E}">
+  <dimension ref="B2:F73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>